<commit_message>
refactor: 将标记从[Config] 改为 [ExcelLENT]
</commit_message>
<xml_diff>
--- a/Test/Excel/测试表.xlsx
+++ b/Test/Excel/测试表.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\ExcelParser\Test\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\ExcelLENT\Test\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FC4852-D1B3-4798-8F15-C683311D1A1F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD99444-08C3-4A2F-971C-28FABCF0299B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="568" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
-    <t>[Config]</t>
-  </si>
-  <si>
     <t>pos</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -137,6 +134,10 @@
   </si>
   <si>
     <t>11;2;3;4;5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[ExcelLENT]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -503,7 +504,7 @@
       <pane xSplit="2" ySplit="8" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -520,70 +521,70 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -595,16 +596,16 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -612,22 +613,22 @@
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>